<commit_message>
Add remove user-role route
</commit_message>
<xml_diff>
--- a/policy_generator/Roles.xlsx
+++ b/policy_generator/Roles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahdi\Git\GitHub\mra-authorization\policy_generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahdi\Git\GitHub\mra-auth\policy_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF94F5B-2829-486F-9E78-06FFF02FAA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACB3275-A332-4260-84DA-D4DBC81B4D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4404" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{252918B9-00B2-423B-B89C-CAD0DFB0D9ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{252918B9-00B2-423B-B89C-CAD0DFB0D9ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="153">
   <si>
     <t>mra_countries</t>
   </si>
@@ -107,9 +107,6 @@
     <t>mra_transition_conditions</t>
   </si>
   <si>
-    <t>mra_ticket_access_levels</t>
-  </si>
-  <si>
     <t>mra_ticket_categories</t>
   </si>
   <si>
@@ -203,9 +200,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>advisor</t>
-  </si>
-  <si>
     <t>enduser</t>
   </si>
   <si>
@@ -419,13 +413,7 @@
     <t>Can read limited rows or under specific conditions (e.g., if related to subscribed customer)</t>
   </si>
   <si>
-    <t>customer_id</t>
-  </si>
-  <si>
     <t>SYS</t>
-  </si>
-  <si>
-    <t>Defines different access levels available for tickets. This table specifies various levels of ticket access, such as public, admins, specific teams, etc., and the roles and permissions needed to access these ticket types.</t>
   </si>
   <si>
     <t>Not allowed to access.</t>
@@ -515,6 +503,21 @@
   </si>
   <si>
     <t>accepted_by</t>
+  </si>
+  <si>
+    <t>C*R*D*</t>
+  </si>
+  <si>
+    <t>CRD</t>
+  </si>
+  <si>
+    <t>C*R*</t>
+  </si>
+  <si>
+    <t>C*RU*D*</t>
+  </si>
+  <si>
+    <t>user_id</t>
   </si>
 </sst>
 </file>
@@ -1420,6 +1423,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1437,15 +1449,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1764,10 +1767,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V60"/>
+  <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,114 +1800,114 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="76" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="103" t="s">
-        <v>119</v>
-      </c>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="105"/>
+        <v>122</v>
+      </c>
+      <c r="B1" s="97" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="99"/>
       <c r="F1" s="75" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="76">
         <v>1</v>
       </c>
-      <c r="B2" s="101" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="102"/>
+      <c r="B2" s="104" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="105"/>
       <c r="F2" s="77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="67">
         <v>2</v>
       </c>
-      <c r="B3" s="97" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="98"/>
+      <c r="B3" s="100" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="101"/>
       <c r="F3" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="67">
         <v>3</v>
       </c>
-      <c r="B4" s="97" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="98"/>
+      <c r="B4" s="100" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="101"/>
       <c r="F4" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="67">
         <v>4</v>
       </c>
-      <c r="B5" s="97" t="s">
-        <v>120</v>
-      </c>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="98"/>
+      <c r="B5" s="100" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="101"/>
       <c r="F5" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="67">
         <v>5</v>
       </c>
-      <c r="B6" s="97" t="s">
-        <v>122</v>
-      </c>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="98"/>
+      <c r="B6" s="100" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="101"/>
       <c r="F6" s="8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="67">
         <v>6</v>
       </c>
-      <c r="B7" s="97" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="97"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="98"/>
+      <c r="B7" s="100" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="101"/>
       <c r="F7" s="31" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="68">
         <v>7</v>
       </c>
-      <c r="B8" s="99" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="100"/>
+      <c r="B8" s="102" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="103"/>
       <c r="F8" s="10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1916,47 +1919,47 @@
       <c r="E10" s="71"/>
       <c r="F10" s="71"/>
       <c r="G10" s="71"/>
-      <c r="H10" s="103" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" s="104"/>
-      <c r="J10" s="104"/>
-      <c r="K10" s="104"/>
-      <c r="L10" s="104"/>
-      <c r="M10" s="104"/>
-      <c r="N10" s="104"/>
-      <c r="O10" s="104"/>
-      <c r="P10" s="104"/>
-      <c r="Q10" s="104"/>
-      <c r="R10" s="104"/>
-      <c r="S10" s="104"/>
-      <c r="T10" s="104"/>
-      <c r="U10" s="105"/>
+      <c r="H10" s="97" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="98"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="98"/>
+      <c r="L10" s="98"/>
+      <c r="M10" s="98"/>
+      <c r="N10" s="98"/>
+      <c r="O10" s="98"/>
+      <c r="P10" s="98"/>
+      <c r="Q10" s="98"/>
+      <c r="R10" s="98"/>
+      <c r="S10" s="98"/>
+      <c r="T10" s="98"/>
+      <c r="U10" s="99"/>
       <c r="V10" s="72"/>
     </row>
     <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="73"/>
-      <c r="H11" s="103" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="104"/>
-      <c r="J11" s="104"/>
-      <c r="K11" s="104"/>
-      <c r="L11" s="104"/>
-      <c r="M11" s="104"/>
-      <c r="N11" s="104"/>
-      <c r="O11" s="105"/>
-      <c r="P11" s="103" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q11" s="104"/>
-      <c r="R11" s="104"/>
-      <c r="S11" s="105"/>
+      <c r="H11" s="97" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="98"/>
+      <c r="N11" s="98"/>
+      <c r="O11" s="99"/>
+      <c r="P11" s="97" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q11" s="98"/>
+      <c r="R11" s="98"/>
+      <c r="S11" s="99"/>
       <c r="T11" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="U11" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="V11" s="74"/>
     </row>
@@ -2008,70 +2011,70 @@
     </row>
     <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B13" s="59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="17" t="s">
-        <v>53</v>
-      </c>
       <c r="I13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="K13" s="11" t="s">
+      <c r="M13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O13" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="L13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="M13" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="N13" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="O13" s="19" t="s">
+      <c r="P13" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="P13" s="25" t="s">
+      <c r="Q13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="Q13" s="11" t="s">
+      <c r="R13" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="R13" s="11" t="s">
+      <c r="S13" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="S13" s="19" t="s">
-        <v>42</v>
-      </c>
       <c r="T13" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="U13" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="V13" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="V13" s="16" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -2079,10 +2082,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="60" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D14" s="53">
         <v>700</v>
@@ -2093,49 +2096,49 @@
       <c r="F14" s="53"/>
       <c r="G14" s="54"/>
       <c r="H14" s="55" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I14" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J14" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K14" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L14" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M14" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N14" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O14" s="57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P14" s="58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q14" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R14" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S14" s="57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T14" s="51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U14" s="55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V14" s="32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -2146,7 +2149,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D15" s="53">
         <v>700</v>
@@ -2157,49 +2160,49 @@
       <c r="F15" s="53"/>
       <c r="G15" s="54"/>
       <c r="H15" s="55" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I15" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J15" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K15" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L15" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M15" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N15" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O15" s="57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P15" s="58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q15" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R15" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S15" s="57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T15" s="51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U15" s="55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V15" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -2207,10 +2210,10 @@
         <v>3</v>
       </c>
       <c r="B16" s="88" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="89" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D16" s="90">
         <v>1</v>
@@ -2221,49 +2224,49 @@
       <c r="F16" s="90"/>
       <c r="G16" s="91"/>
       <c r="H16" s="92" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I16" s="93" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J16" s="93" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K16" s="93" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L16" s="93" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M16" s="93" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N16" s="93" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O16" s="94" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P16" s="95" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q16" s="93" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R16" s="93" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S16" s="94" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T16" s="96" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="U16" s="92" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V16" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -2271,10 +2274,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="88" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="89" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D17" s="90">
         <v>1</v>
@@ -2285,49 +2288,49 @@
       <c r="F17" s="90"/>
       <c r="G17" s="91"/>
       <c r="H17" s="92" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I17" s="93" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J17" s="93" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K17" s="93" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L17" s="93" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M17" s="93" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N17" s="93" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O17" s="94" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P17" s="95" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Q17" s="93" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="R17" s="93" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S17" s="94" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="T17" s="96" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="U17" s="92" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V17" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -2338,7 +2341,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D18" s="38">
         <v>1</v>
@@ -2349,49 +2352,49 @@
       <c r="F18" s="38"/>
       <c r="G18" s="39"/>
       <c r="H18" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I18" s="41" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J18" s="41" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K18" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L18" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M18" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N18" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O18" s="42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P18" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q18" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R18" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S18" s="42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T18" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U18" s="40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V18" s="33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
@@ -2402,7 +2405,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D19" s="45">
         <v>1</v>
@@ -2413,49 +2416,49 @@
       <c r="F19" s="45"/>
       <c r="G19" s="46"/>
       <c r="H19" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I19" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J19" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K19" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L19" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M19" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N19" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O19" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P19" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q19" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R19" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S19" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T19" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U19" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V19" s="33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
@@ -2463,10 +2466,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="62" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D20" s="45">
         <v>1</v>
@@ -2477,49 +2480,49 @@
       <c r="F20" s="45"/>
       <c r="G20" s="46"/>
       <c r="H20" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I20" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J20" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K20" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L20" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M20" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N20" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O20" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P20" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q20" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R20" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S20" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T20" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U20" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V20" s="33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -2530,7 +2533,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D21" s="45">
         <v>1</v>
@@ -2541,49 +2544,49 @@
       <c r="F21" s="45"/>
       <c r="G21" s="46"/>
       <c r="H21" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I21" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J21" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K21" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L21" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M21" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N21" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O21" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P21" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q21" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R21" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S21" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T21" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U21" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V21" s="33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
@@ -2594,7 +2597,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D22" s="45">
         <v>100</v>
@@ -2605,49 +2608,49 @@
       <c r="F22" s="45"/>
       <c r="G22" s="46"/>
       <c r="H22" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I22" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J22" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K22" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L22" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M22" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N22" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O22" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P22" s="50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q22" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R22" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S22" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T22" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U22" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V22" s="33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
@@ -2658,7 +2661,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D23" s="45">
         <v>1</v>
@@ -2669,49 +2672,49 @@
       <c r="F23" s="45"/>
       <c r="G23" s="46"/>
       <c r="H23" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I23" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J23" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K23" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L23" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M23" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N23" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O23" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P23" s="50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q23" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R23" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S23" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T23" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U23" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V23" s="33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -2722,7 +2725,7 @@
         <v>15</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D24" s="45">
         <v>1</v>
@@ -2733,49 +2736,49 @@
       <c r="F24" s="45"/>
       <c r="G24" s="46"/>
       <c r="H24" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I24" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J24" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K24" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L24" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M24" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N24" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O24" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P24" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q24" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R24" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S24" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T24" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U24" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V24" s="33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -2786,7 +2789,7 @@
         <v>16</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D25" s="45">
         <v>1</v>
@@ -2797,49 +2800,49 @@
       <c r="F25" s="45"/>
       <c r="G25" s="46"/>
       <c r="H25" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I25" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J25" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K25" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L25" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M25" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N25" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O25" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P25" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q25" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R25" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S25" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T25" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U25" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V25" s="33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -2850,7 +2853,7 @@
         <v>20</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D26" s="45">
         <v>1</v>
@@ -2861,49 +2864,49 @@
       <c r="F26" s="45"/>
       <c r="G26" s="46"/>
       <c r="H26" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I26" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J26" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K26" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L26" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M26" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N26" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O26" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P26" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q26" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R26" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S26" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T26" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U26" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V26" s="33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
@@ -2911,10 +2914,10 @@
         <v>14</v>
       </c>
       <c r="B27" s="62" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D27" s="45">
         <v>1</v>
@@ -2925,49 +2928,49 @@
       <c r="F27" s="45"/>
       <c r="G27" s="46"/>
       <c r="H27" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I27" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J27" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K27" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L27" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M27" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N27" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O27" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P27" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q27" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R27" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S27" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T27" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U27" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V27" s="33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
@@ -2975,10 +2978,10 @@
         <v>15</v>
       </c>
       <c r="B28" s="62" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D28" s="45">
         <v>900</v>
@@ -2989,49 +2992,49 @@
       <c r="F28" s="45"/>
       <c r="G28" s="46"/>
       <c r="H28" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I28" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J28" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K28" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L28" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M28" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N28" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O28" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P28" s="50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q28" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R28" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S28" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T28" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U28" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V28" s="33" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
@@ -3042,7 +3045,7 @@
         <v>10</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D29" s="45">
         <v>80</v>
@@ -3053,49 +3056,49 @@
       <c r="F29" s="45"/>
       <c r="G29" s="46"/>
       <c r="H29" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I29" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J29" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K29" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L29" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M29" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N29" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O29" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P29" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q29" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R29" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S29" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T29" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U29" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V29" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
@@ -3103,10 +3106,10 @@
         <v>17</v>
       </c>
       <c r="B30" s="62" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D30" s="45">
         <v>80</v>
@@ -3117,49 +3120,49 @@
       <c r="F30" s="45"/>
       <c r="G30" s="46"/>
       <c r="H30" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I30" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J30" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K30" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L30" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M30" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N30" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O30" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P30" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q30" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R30" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S30" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T30" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U30" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V30" s="33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
@@ -3167,10 +3170,10 @@
         <v>18</v>
       </c>
       <c r="B31" s="62" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D31" s="45">
         <v>80</v>
@@ -3181,49 +3184,49 @@
       <c r="F31" s="45"/>
       <c r="G31" s="46"/>
       <c r="H31" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I31" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J31" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K31" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L31" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M31" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="N31" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O31" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P31" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q31" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R31" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S31" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T31" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U31" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V31" s="33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
@@ -3231,10 +3234,10 @@
         <v>19</v>
       </c>
       <c r="B32" s="62" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D32" s="45">
         <v>80</v>
@@ -3245,49 +3248,49 @@
       <c r="F32" s="45"/>
       <c r="G32" s="46"/>
       <c r="H32" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I32" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J32" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K32" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L32" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M32" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="N32" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O32" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P32" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q32" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R32" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S32" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T32" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U32" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V32" s="33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
@@ -3295,10 +3298,10 @@
         <v>20</v>
       </c>
       <c r="B33" s="62" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D33" s="45">
         <v>80</v>
@@ -3309,49 +3312,49 @@
       <c r="F33" s="45"/>
       <c r="G33" s="46"/>
       <c r="H33" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I33" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J33" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K33" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L33" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M33" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="N33" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O33" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P33" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q33" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R33" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S33" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T33" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U33" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V33" s="33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
@@ -3362,7 +3365,7 @@
         <v>6</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D34" s="45">
         <v>80</v>
@@ -3373,49 +3376,49 @@
       <c r="F34" s="45"/>
       <c r="G34" s="46"/>
       <c r="H34" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I34" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J34" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K34" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L34" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M34" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="N34" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O34" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P34" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q34" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R34" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S34" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T34" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U34" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V34" s="33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
@@ -3426,7 +3429,7 @@
         <v>7</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D35" s="45">
         <v>80</v>
@@ -3437,49 +3440,49 @@
       <c r="F35" s="45"/>
       <c r="G35" s="46"/>
       <c r="H35" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I35" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J35" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K35" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L35" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M35" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="N35" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O35" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P35" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q35" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R35" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S35" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T35" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U35" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V35" s="33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
@@ -3490,7 +3493,7 @@
         <v>8</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D36" s="45">
         <v>80</v>
@@ -3501,49 +3504,49 @@
       <c r="F36" s="45"/>
       <c r="G36" s="46"/>
       <c r="H36" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I36" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J36" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K36" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L36" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M36" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="N36" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O36" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P36" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q36" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R36" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S36" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T36" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U36" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V36" s="33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
@@ -3551,10 +3554,10 @@
         <v>24</v>
       </c>
       <c r="B37" s="62" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D37" s="45">
         <v>80</v>
@@ -3565,49 +3568,49 @@
       <c r="F37" s="45"/>
       <c r="G37" s="46"/>
       <c r="H37" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I37" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J37" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K37" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L37" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M37" s="48" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="N37" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O37" s="49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P37" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q37" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R37" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S37" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T37" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U37" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V37" s="33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
@@ -3618,7 +3621,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="D38" s="26">
         <v>1</v>
@@ -3630,52 +3633,52 @@
         <v>100</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H38" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O38" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="I38" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N38" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="O38" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="P38" s="21" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="T38" s="13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="U38" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V38" s="33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
@@ -3686,7 +3689,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="D39" s="26">
         <v>100</v>
@@ -3697,49 +3700,49 @@
       <c r="F39" s="26"/>
       <c r="G39" s="27"/>
       <c r="H39" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P39" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T39" s="13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="U39" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V39" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
@@ -3750,7 +3753,7 @@
         <v>18</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D40" s="26">
         <v>100</v>
@@ -3761,49 +3764,49 @@
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
       <c r="H40" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P40" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S40" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T40" s="13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="U40" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V40" s="33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
@@ -3811,10 +3814,10 @@
         <v>28</v>
       </c>
       <c r="B41" s="63" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D41" s="26">
         <v>1</v>
@@ -3824,52 +3827,52 @@
       </c>
       <c r="F41" s="26"/>
       <c r="G41" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H41" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P41" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S41" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T41" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U41" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V41" s="33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
@@ -3877,10 +3880,10 @@
         <v>29</v>
       </c>
       <c r="B42" s="64" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="D42" s="7">
         <v>20</v>
@@ -3891,49 +3894,49 @@
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
       <c r="H42" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="P42" s="21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S42" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="T42" s="13" t="s">
-        <v>54</v>
+        <v>138</v>
       </c>
       <c r="U42" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V42" s="33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
@@ -3944,7 +3947,7 @@
         <v>9</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D43" s="26">
         <v>80</v>
@@ -3955,49 +3958,49 @@
       <c r="F43" s="26"/>
       <c r="G43" s="27"/>
       <c r="H43" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P43" s="21" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R43" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T43" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U43" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V43" s="33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
@@ -4008,7 +4011,7 @@
         <v>11</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D44" s="26">
         <v>80</v>
@@ -4019,49 +4022,49 @@
       <c r="F44" s="26"/>
       <c r="G44" s="27"/>
       <c r="H44" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P44" s="21" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T44" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U44" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V44" s="33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
@@ -4072,7 +4075,7 @@
         <v>14</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D45" s="26">
         <v>1</v>
@@ -4083,49 +4086,49 @@
       <c r="F45" s="26"/>
       <c r="G45" s="27"/>
       <c r="H45" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P45" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S45" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T45" s="13" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="U45" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V45" s="33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
@@ -4136,7 +4139,7 @@
         <v>17</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D46" s="7">
         <v>1</v>
@@ -4147,49 +4150,49 @@
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
       <c r="H46" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="P46" s="21" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="Q46" s="2" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S46" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="T46" s="13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="U46" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V46" s="33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
@@ -4197,10 +4200,10 @@
         <v>34</v>
       </c>
       <c r="B47" s="64" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="D47" s="7">
         <v>50</v>
@@ -4211,49 +4214,49 @@
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
       <c r="H47" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O47" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P47" s="21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="R47" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T47" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U47" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V47" s="33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
@@ -4264,7 +4267,7 @@
         <v>19</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="D48" s="7">
         <v>1</v>
@@ -4275,49 +4278,49 @@
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
       <c r="H48" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P48" s="21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="R48" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="T48" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U48" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V48" s="33" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
@@ -4328,7 +4331,7 @@
         <v>21</v>
       </c>
       <c r="C49" s="29" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="D49" s="7">
         <v>20</v>
@@ -4339,49 +4342,49 @@
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
       <c r="H49" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P49" s="21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S49" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="T49" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U49" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V49" s="33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
@@ -4392,7 +4395,7 @@
         <v>22</v>
       </c>
       <c r="C50" s="29" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="D50" s="7">
         <v>20</v>
@@ -4403,49 +4406,49 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
       <c r="H50" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P50" s="21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="Q50" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="R50" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S50" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="T50" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U50" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V50" s="33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
@@ -4456,7 +4459,7 @@
         <v>23</v>
       </c>
       <c r="C51" s="29" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="D51" s="7">
         <v>1</v>
@@ -4467,49 +4470,49 @@
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
       <c r="H51" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="P51" s="21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="R51" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S51" s="3" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="T51" s="13" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="U51" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V51" s="33" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
@@ -4520,60 +4523,60 @@
         <v>24</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="D52" s="7">
+        <v>0</v>
+      </c>
+      <c r="E52" s="7">
         <v>1</v>
-      </c>
-      <c r="E52" s="7">
-        <v>60</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
       <c r="H52" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
       <c r="O52" s="3" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
       <c r="P52" s="21" t="s">
-        <v>148</v>
+        <v>46</v>
       </c>
       <c r="Q52" s="2" t="s">
-        <v>148</v>
+        <v>46</v>
       </c>
       <c r="R52" s="2" t="s">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="S52" s="3" t="s">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="T52" s="13" t="s">
-        <v>47</v>
+        <v>135</v>
       </c>
       <c r="U52" s="23" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="V52" s="33" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
@@ -4584,60 +4587,60 @@
         <v>25</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D53" s="7">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E53" s="7">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
       <c r="H53" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O53" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P53" s="21" t="s">
-        <v>47</v>
+        <v>144</v>
       </c>
       <c r="Q53" s="2" t="s">
-        <v>47</v>
+        <v>136</v>
       </c>
       <c r="R53" s="2" t="s">
-        <v>47</v>
+        <v>136</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
       <c r="T53" s="13" t="s">
-        <v>139</v>
+        <v>53</v>
       </c>
       <c r="U53" s="23" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="V53" s="33" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
@@ -4645,63 +4648,63 @@
         <v>41</v>
       </c>
       <c r="B54" s="64" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="D54" s="7">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E54" s="7">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
       <c r="H54" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P54" s="21" t="s">
-        <v>148</v>
+        <v>46</v>
       </c>
       <c r="Q54" s="2" t="s">
-        <v>148</v>
+        <v>46</v>
       </c>
       <c r="R54" s="2" t="s">
-        <v>140</v>
+        <v>46</v>
       </c>
       <c r="S54" s="3" t="s">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="T54" s="13" t="s">
-        <v>54</v>
+        <v>135</v>
       </c>
       <c r="U54" s="23" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="V54" s="33" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
@@ -4712,7 +4715,7 @@
         <v>28</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D55" s="7">
         <v>1</v>
@@ -4723,344 +4726,280 @@
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
       <c r="H55" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P55" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q55" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R55" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T55" s="13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="U55" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V55" s="33" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="79">
         <v>43</v>
       </c>
-      <c r="B56" s="64" t="s">
-        <v>29</v>
+      <c r="B56" s="65" t="s">
+        <v>64</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D56" s="7">
-        <v>1</v>
-      </c>
-      <c r="E56" s="7">
-        <v>1</v>
-      </c>
-      <c r="F56" s="7"/>
-      <c r="G56" s="8"/>
+        <v>47</v>
+      </c>
+      <c r="D56" s="30">
+        <v>40</v>
+      </c>
+      <c r="E56" s="30">
+        <v>600</v>
+      </c>
+      <c r="F56" s="30"/>
+      <c r="G56" s="31"/>
       <c r="H56" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>47</v>
+        <v>133</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>47</v>
+        <v>133</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P56" s="21" t="s">
-        <v>47</v>
+        <v>142</v>
       </c>
       <c r="Q56" s="2" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="S56" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="T56" s="13" t="s">
-        <v>139</v>
+        <v>53</v>
       </c>
       <c r="U56" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="V56" s="33" t="s">
-        <v>107</v>
+        <v>53</v>
+      </c>
+      <c r="V56" s="34" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="79">
         <v>44</v>
       </c>
-      <c r="B57" s="65" t="s">
-        <v>66</v>
+      <c r="B57" s="64" t="s">
+        <v>107</v>
       </c>
       <c r="C57" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D57" s="30">
-        <v>40</v>
-      </c>
-      <c r="E57" s="30">
-        <v>600</v>
-      </c>
-      <c r="F57" s="30"/>
-      <c r="G57" s="31"/>
+        <v>47</v>
+      </c>
+      <c r="D57" s="7">
+        <v>0</v>
+      </c>
+      <c r="E57" s="7">
+        <v>60</v>
+      </c>
+      <c r="F57" s="7"/>
+      <c r="G57" s="8"/>
       <c r="H57" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O57" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P57" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q57" s="2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="R57" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="S57" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="T57" s="13" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="U57" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="V57" s="34" t="s">
-        <v>132</v>
+        <v>46</v>
+      </c>
+      <c r="V57" s="33" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="79">
         <v>45</v>
       </c>
-      <c r="B58" s="64" t="s">
-        <v>109</v>
-      </c>
-      <c r="C58" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="D58" s="7">
-        <v>0</v>
-      </c>
-      <c r="E58" s="7">
-        <v>60</v>
-      </c>
-      <c r="F58" s="7"/>
-      <c r="G58" s="8"/>
+      <c r="B58" s="65" t="s">
+        <v>140</v>
+      </c>
+      <c r="C58" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="D58" s="30">
+        <v>700</v>
+      </c>
+      <c r="E58" s="30">
+        <v>800</v>
+      </c>
+      <c r="F58" s="30"/>
+      <c r="G58" s="31"/>
       <c r="H58" s="23" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M58" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N58" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="O58" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="P58" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="Q58" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="R58" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="S58" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="T58" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="U58" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="V58" s="33" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A59" s="79">
-        <v>46</v>
-      </c>
-      <c r="B59" s="65" t="s">
-        <v>144</v>
-      </c>
-      <c r="C59" s="82" t="s">
-        <v>128</v>
-      </c>
-      <c r="D59" s="30">
-        <v>700</v>
-      </c>
-      <c r="E59" s="30">
-        <v>800</v>
-      </c>
-      <c r="F59" s="30"/>
-      <c r="G59" s="31"/>
-      <c r="H59" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="J59" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="K59" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="L59" s="84" t="s">
-        <v>47</v>
-      </c>
-      <c r="M59" s="84" t="s">
-        <v>54</v>
-      </c>
-      <c r="N59" s="84" t="s">
-        <v>54</v>
-      </c>
-      <c r="O59" s="85" t="s">
-        <v>54</v>
-      </c>
-      <c r="P59" s="86" t="s">
+      <c r="L58" s="84" t="s">
+        <v>46</v>
+      </c>
+      <c r="M58" s="84" t="s">
+        <v>53</v>
+      </c>
+      <c r="N58" s="84" t="s">
+        <v>53</v>
+      </c>
+      <c r="O58" s="85" t="s">
+        <v>53</v>
+      </c>
+      <c r="P58" s="86" t="s">
         <v>148</v>
       </c>
-      <c r="Q59" s="84" t="s">
-        <v>54</v>
-      </c>
-      <c r="R59" s="84" t="s">
-        <v>54</v>
-      </c>
-      <c r="S59" s="85" t="s">
-        <v>54</v>
-      </c>
-      <c r="T59" s="87" t="s">
-        <v>54</v>
-      </c>
-      <c r="U59" s="83" t="s">
-        <v>54</v>
-      </c>
-      <c r="V59" s="34" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="60" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="80"/>
-      <c r="B60" s="66"/>
-      <c r="C60" s="81"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="10"/>
-      <c r="H60" s="24"/>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
-      <c r="O60" s="5"/>
-      <c r="P60" s="22"/>
-      <c r="Q60" s="4"/>
-      <c r="R60" s="4"/>
-      <c r="S60" s="5"/>
-      <c r="T60" s="6"/>
-      <c r="U60" s="24"/>
-      <c r="V60" s="35"/>
+      <c r="Q58" s="84" t="s">
+        <v>53</v>
+      </c>
+      <c r="R58" s="84" t="s">
+        <v>53</v>
+      </c>
+      <c r="S58" s="85" t="s">
+        <v>53</v>
+      </c>
+      <c r="T58" s="87" t="s">
+        <v>53</v>
+      </c>
+      <c r="U58" s="83" t="s">
+        <v>53</v>
+      </c>
+      <c r="V58" s="34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="80"/>
+      <c r="B59" s="66"/>
+      <c r="C59" s="81"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="5"/>
+      <c r="P59" s="22"/>
+      <c r="Q59" s="4"/>
+      <c r="R59" s="4"/>
+      <c r="S59" s="5"/>
+      <c r="T59" s="6"/>
+      <c r="U59" s="24"/>
+      <c r="V59" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="H11:O11"/>
     <mergeCell ref="P11:S11"/>
     <mergeCell ref="H10:U10"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="35" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Add more policy and role route
</commit_message>
<xml_diff>
--- a/policy_generator/Roles.xlsx
+++ b/policy_generator/Roles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahdi\Git\GitHub\mra-auth\policy_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACB3275-A332-4260-84DA-D4DBC81B4D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0C872E-8BBD-43CA-B2CA-2DE87CD90F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{252918B9-00B2-423B-B89C-CAD0DFB0D9ED}"/>
   </bookViews>
@@ -481,9 +481,6 @@
     <t>CUD</t>
   </si>
   <si>
-    <t>casbin_rule</t>
-  </si>
-  <si>
     <t xml:space="preserve">A casbin table for managing roles and only modifiable via authorization service. </t>
   </si>
   <si>
@@ -518,6 +515,9 @@
   </si>
   <si>
     <t>user_id</t>
+  </si>
+  <si>
+    <t>mra_authorization</t>
   </si>
 </sst>
 </file>
@@ -1423,15 +1423,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1449,6 +1440,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1770,7 +1770,7 @@
   <dimension ref="A1:V59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,12 +1802,12 @@
       <c r="A1" s="76" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="103" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="99"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="105"/>
       <c r="F1" s="75" t="s">
         <v>131</v>
       </c>
@@ -1816,12 +1816,12 @@
       <c r="A2" s="76">
         <v>1</v>
       </c>
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="101" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="105"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="102"/>
       <c r="F2" s="77" t="s">
         <v>53</v>
       </c>
@@ -1830,12 +1830,12 @@
       <c r="A3" s="67">
         <v>2</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="97" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="101"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="98"/>
       <c r="F3" s="8" t="s">
         <v>46</v>
       </c>
@@ -1844,12 +1844,12 @@
       <c r="A4" s="67">
         <v>3</v>
       </c>
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="97" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="101"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="98"/>
       <c r="F4" s="8" t="s">
         <v>116</v>
       </c>
@@ -1858,12 +1858,12 @@
       <c r="A5" s="67">
         <v>4</v>
       </c>
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="97" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="101"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="98"/>
       <c r="F5" s="8" t="s">
         <v>135</v>
       </c>
@@ -1872,12 +1872,12 @@
       <c r="A6" s="67">
         <v>5</v>
       </c>
-      <c r="B6" s="100" t="s">
+      <c r="B6" s="97" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="101"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="98"/>
       <c r="F6" s="8" t="s">
         <v>139</v>
       </c>
@@ -1886,12 +1886,12 @@
       <c r="A7" s="67">
         <v>6</v>
       </c>
-      <c r="B7" s="100" t="s">
+      <c r="B7" s="97" t="s">
         <v>121</v>
       </c>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="101"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="98"/>
       <c r="F7" s="31" t="s">
         <v>133</v>
       </c>
@@ -1900,12 +1900,12 @@
       <c r="A8" s="68">
         <v>7</v>
       </c>
-      <c r="B8" s="102" t="s">
+      <c r="B8" s="99" t="s">
         <v>123</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="103"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="99"/>
+      <c r="E8" s="100"/>
       <c r="F8" s="10" t="s">
         <v>134</v>
       </c>
@@ -1919,42 +1919,42 @@
       <c r="E10" s="71"/>
       <c r="F10" s="71"/>
       <c r="G10" s="71"/>
-      <c r="H10" s="97" t="s">
+      <c r="H10" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="98"/>
-      <c r="J10" s="98"/>
-      <c r="K10" s="98"/>
-      <c r="L10" s="98"/>
-      <c r="M10" s="98"/>
-      <c r="N10" s="98"/>
-      <c r="O10" s="98"/>
-      <c r="P10" s="98"/>
-      <c r="Q10" s="98"/>
-      <c r="R10" s="98"/>
-      <c r="S10" s="98"/>
-      <c r="T10" s="98"/>
-      <c r="U10" s="99"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="104"/>
+      <c r="L10" s="104"/>
+      <c r="M10" s="104"/>
+      <c r="N10" s="104"/>
+      <c r="O10" s="104"/>
+      <c r="P10" s="104"/>
+      <c r="Q10" s="104"/>
+      <c r="R10" s="104"/>
+      <c r="S10" s="104"/>
+      <c r="T10" s="104"/>
+      <c r="U10" s="105"/>
       <c r="V10" s="72"/>
     </row>
     <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="73"/>
-      <c r="H11" s="97" t="s">
+      <c r="H11" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="I11" s="98"/>
-      <c r="J11" s="98"/>
-      <c r="K11" s="98"/>
-      <c r="L11" s="98"/>
-      <c r="M11" s="98"/>
-      <c r="N11" s="98"/>
-      <c r="O11" s="99"/>
-      <c r="P11" s="97" t="s">
+      <c r="I11" s="104"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="104"/>
+      <c r="L11" s="104"/>
+      <c r="M11" s="104"/>
+      <c r="N11" s="104"/>
+      <c r="O11" s="105"/>
+      <c r="P11" s="103" t="s">
         <v>130</v>
       </c>
-      <c r="Q11" s="98"/>
-      <c r="R11" s="98"/>
-      <c r="S11" s="99"/>
+      <c r="Q11" s="104"/>
+      <c r="R11" s="104"/>
+      <c r="S11" s="105"/>
       <c r="T11" s="14" t="s">
         <v>55</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D38" s="26">
         <v>1</v>
@@ -3660,10 +3660,10 @@
         <v>137</v>
       </c>
       <c r="P38" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R38" s="2" t="s">
         <v>116</v>
@@ -3689,7 +3689,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D39" s="26">
         <v>100</v>
@@ -3883,7 +3883,7 @@
         <v>78</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D42" s="7">
         <v>20</v>
@@ -3918,7 +3918,7 @@
         <v>133</v>
       </c>
       <c r="P42" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q42" s="2" t="s">
         <v>136</v>
@@ -3982,7 +3982,7 @@
         <v>46</v>
       </c>
       <c r="P43" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Q43" s="2" t="s">
         <v>53</v>
@@ -4046,7 +4046,7 @@
         <v>46</v>
       </c>
       <c r="P44" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Q44" s="2" t="s">
         <v>53</v>
@@ -4075,7 +4075,7 @@
         <v>14</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D45" s="26">
         <v>1</v>
@@ -4122,7 +4122,7 @@
         <v>53</v>
       </c>
       <c r="T45" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U45" s="23" t="s">
         <v>53</v>
@@ -4174,7 +4174,7 @@
         <v>133</v>
       </c>
       <c r="P46" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Q46" s="2" t="s">
         <v>116</v>
@@ -4238,7 +4238,7 @@
         <v>46</v>
       </c>
       <c r="P47" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q47" s="2" t="s">
         <v>136</v>
@@ -4302,7 +4302,7 @@
         <v>46</v>
       </c>
       <c r="P48" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q48" s="2" t="s">
         <v>136</v>
@@ -4366,7 +4366,7 @@
         <v>46</v>
       </c>
       <c r="P49" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q49" s="2" t="s">
         <v>136</v>
@@ -4430,7 +4430,7 @@
         <v>46</v>
       </c>
       <c r="P50" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>136</v>
@@ -4494,7 +4494,7 @@
         <v>133</v>
       </c>
       <c r="P51" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q51" s="2" t="s">
         <v>136</v>
@@ -4622,7 +4622,7 @@
         <v>46</v>
       </c>
       <c r="P53" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q53" s="2" t="s">
         <v>136</v>
@@ -4814,7 +4814,7 @@
         <v>46</v>
       </c>
       <c r="P56" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Q56" s="2" t="s">
         <v>116</v>
@@ -4878,10 +4878,10 @@
         <v>46</v>
       </c>
       <c r="P57" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Q57" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R57" s="2" t="s">
         <v>46</v>
@@ -4904,7 +4904,7 @@
         <v>45</v>
       </c>
       <c r="B58" s="65" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="C58" s="82" t="s">
         <v>125</v>
@@ -4918,16 +4918,16 @@
       <c r="F58" s="30"/>
       <c r="G58" s="31"/>
       <c r="H58" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L58" s="84" t="s">
         <v>46</v>
@@ -4942,7 +4942,7 @@
         <v>53</v>
       </c>
       <c r="P58" s="86" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Q58" s="84" t="s">
         <v>53</v>
@@ -4960,7 +4960,7 @@
         <v>53</v>
       </c>
       <c r="V58" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4989,17 +4989,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="H11:O11"/>
     <mergeCell ref="P11:S11"/>
     <mergeCell ref="H10:U10"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="35" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Update on policy to support s3-files also
</commit_message>
<xml_diff>
--- a/policy_generator/Roles.xlsx
+++ b/policy_generator/Roles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahdi\Git\GitHub\mra-auth\policy_generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahdijaberzadehansari/GitHub/mra-auth/policy_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0C872E-8BBD-43CA-B2CA-2DE87CD90F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF72304-DC3B-C741-8786-6C5E55EA2E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{252918B9-00B2-423B-B89C-CAD0DFB0D9ED}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="15840" xr2:uid="{252918B9-00B2-423B-B89C-CAD0DFB0D9ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="158">
   <si>
     <t>mra_countries</t>
   </si>
@@ -363,9 +363,6 @@
   </si>
   <si>
     <t>Manages post items or updates that may be related to tickets or system updates. This table includes various posts content with geospatial data and time-related publication settings.</t>
-  </si>
-  <si>
-    <t>mra_discount_type</t>
   </si>
   <si>
     <t>This table stores the different types of discounts available. Each discount type is uniquely identified and classified by its name, which indicates whether it is a percentage-based discount or a fixed value discount.</t>
@@ -518,6 +515,24 @@
   </si>
   <si>
     <t>mra_authorization</t>
+  </si>
+  <si>
+    <t>CORUODO</t>
+  </si>
+  <si>
+    <t>mra_audit_logs_core</t>
+  </si>
+  <si>
+    <t>mra_audit_logs_file</t>
+  </si>
+  <si>
+    <t>s3_files</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>mra_discount_types</t>
   </si>
 </sst>
 </file>
@@ -1391,9 +1406,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1423,6 +1435,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1767,57 +1780,57 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V59"/>
+  <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" customWidth="1"/>
-    <col min="17" max="17" width="21.28515625" customWidth="1"/>
-    <col min="18" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" customWidth="1"/>
-    <col min="21" max="21" width="11.85546875" customWidth="1"/>
-    <col min="22" max="22" width="255.5703125" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.1640625" customWidth="1"/>
+    <col min="17" max="17" width="21.33203125" customWidth="1"/>
+    <col min="18" max="19" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5" customWidth="1"/>
+    <col min="21" max="21" width="11.83203125" customWidth="1"/>
+    <col min="22" max="22" width="255.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="76" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="103" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C1" s="104"/>
       <c r="D1" s="104"/>
       <c r="E1" s="105"/>
       <c r="F1" s="75" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="76">
         <v>1</v>
       </c>
       <c r="B2" s="101" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="101"/>
       <c r="D2" s="101"/>
@@ -1826,12 +1839,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="67">
         <v>2</v>
       </c>
       <c r="B3" s="97" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" s="97"/>
       <c r="D3" s="97"/>
@@ -1840,78 +1853,78 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="67">
         <v>3</v>
       </c>
       <c r="B4" s="97" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" s="97"/>
       <c r="D4" s="97"/>
       <c r="E4" s="98"/>
       <c r="F4" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="67">
         <v>4</v>
       </c>
       <c r="B5" s="97" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" s="97"/>
       <c r="D5" s="97"/>
       <c r="E5" s="98"/>
       <c r="F5" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="67">
         <v>5</v>
       </c>
       <c r="B6" s="97" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" s="97"/>
       <c r="D6" s="97"/>
       <c r="E6" s="98"/>
       <c r="F6" s="8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="67">
         <v>6</v>
       </c>
       <c r="B7" s="97" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" s="97"/>
       <c r="D7" s="97"/>
       <c r="E7" s="98"/>
       <c r="F7" s="31" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="68">
         <v>7</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="99"/>
       <c r="D8" s="99"/>
       <c r="E8" s="100"/>
       <c r="F8" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="69"/>
       <c r="B10" s="70"/>
       <c r="C10" s="71"/>
@@ -1937,7 +1950,7 @@
       <c r="U10" s="105"/>
       <c r="V10" s="72"/>
     </row>
-    <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="73"/>
       <c r="H11" s="103" t="s">
         <v>57</v>
@@ -1950,7 +1963,7 @@
       <c r="N11" s="104"/>
       <c r="O11" s="105"/>
       <c r="P11" s="103" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q11" s="104"/>
       <c r="R11" s="104"/>
@@ -1963,7 +1976,7 @@
       </c>
       <c r="V11" s="74"/>
     </row>
-    <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="73"/>
       <c r="H12" s="17">
         <v>1100</v>
@@ -2009,7 +2022,7 @@
       </c>
       <c r="V12" s="74"/>
     </row>
-    <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>91</v>
       </c>
@@ -2017,7 +2030,7 @@
         <v>45</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>44</v>
@@ -2077,15 +2090,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="78">
         <v>1</v>
       </c>
       <c r="B14" s="60" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D14" s="53">
         <v>700</v>
@@ -2096,7 +2109,7 @@
       <c r="F14" s="53"/>
       <c r="G14" s="54"/>
       <c r="H14" s="55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I14" s="56" t="s">
         <v>46</v>
@@ -2138,18 +2151,18 @@
         <v>53</v>
       </c>
       <c r="V14" s="32" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="79">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" s="78">
         <v>2</v>
       </c>
       <c r="B15" s="60" t="s">
-        <v>5</v>
+        <v>153</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D15" s="53">
         <v>700</v>
@@ -2160,7 +2173,7 @@
       <c r="F15" s="53"/>
       <c r="G15" s="54"/>
       <c r="H15" s="55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I15" s="56" t="s">
         <v>46</v>
@@ -2201,339 +2214,335 @@
       <c r="U15" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="V15" s="33" t="s">
+      <c r="V15" s="96"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" s="78">
+        <v>3</v>
+      </c>
+      <c r="B16" s="60" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="53">
+        <v>700</v>
+      </c>
+      <c r="E16" s="53">
+        <v>1100</v>
+      </c>
+      <c r="F16" s="53"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="I16" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="K16" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="M16" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="N16" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="O16" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="P16" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q16" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="R16" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="S16" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="T16" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="U16" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="V16" s="96"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17" s="78">
+        <v>4</v>
+      </c>
+      <c r="B17" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" s="53">
+        <v>700</v>
+      </c>
+      <c r="E17" s="53">
+        <v>1100</v>
+      </c>
+      <c r="F17" s="53"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="I17" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="L17" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="M17" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="N17" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="O17" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="P17" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q17" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="R17" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="S17" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="T17" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="U17" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="V17" s="33" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="79">
-        <v>3</v>
-      </c>
-      <c r="B16" s="88" t="s">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A18" s="78">
+        <v>5</v>
+      </c>
+      <c r="B18" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="89" t="s">
-        <v>125</v>
-      </c>
-      <c r="D16" s="90">
+      <c r="C18" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="89">
         <v>1</v>
       </c>
-      <c r="E16" s="90">
+      <c r="E18" s="89">
         <v>1100</v>
       </c>
-      <c r="F16" s="90"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="92" t="s">
-        <v>133</v>
-      </c>
-      <c r="I16" s="93" t="s">
-        <v>46</v>
-      </c>
-      <c r="J16" s="93" t="s">
-        <v>46</v>
-      </c>
-      <c r="K16" s="93" t="s">
-        <v>53</v>
-      </c>
-      <c r="L16" s="93" t="s">
-        <v>53</v>
-      </c>
-      <c r="M16" s="93" t="s">
-        <v>53</v>
-      </c>
-      <c r="N16" s="93" t="s">
-        <v>53</v>
-      </c>
-      <c r="O16" s="94" t="s">
-        <v>53</v>
-      </c>
-      <c r="P16" s="95" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q16" s="93" t="s">
-        <v>53</v>
-      </c>
-      <c r="R16" s="93" t="s">
-        <v>53</v>
-      </c>
-      <c r="S16" s="94" t="s">
-        <v>53</v>
-      </c>
-      <c r="T16" s="96" t="s">
-        <v>132</v>
-      </c>
-      <c r="U16" s="92" t="s">
-        <v>53</v>
-      </c>
-      <c r="V16" s="33" t="s">
+      <c r="F18" s="89"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="91" t="s">
+        <v>132</v>
+      </c>
+      <c r="I18" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="K18" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="L18" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="N18" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="O18" s="93" t="s">
+        <v>53</v>
+      </c>
+      <c r="P18" s="94" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q18" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="R18" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="S18" s="93" t="s">
+        <v>53</v>
+      </c>
+      <c r="T18" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="U18" s="91" t="s">
+        <v>53</v>
+      </c>
+      <c r="V18" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="79">
-        <v>4</v>
-      </c>
-      <c r="B17" s="88" t="s">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A19" s="78">
+        <v>6</v>
+      </c>
+      <c r="B19" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="89" t="s">
-        <v>125</v>
-      </c>
-      <c r="D17" s="90">
+      <c r="C19" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="89">
         <v>1</v>
       </c>
-      <c r="E17" s="90">
+      <c r="E19" s="89">
         <v>1100</v>
       </c>
-      <c r="F17" s="90"/>
-      <c r="G17" s="91"/>
-      <c r="H17" s="92" t="s">
-        <v>133</v>
-      </c>
-      <c r="I17" s="93" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="93" t="s">
-        <v>46</v>
-      </c>
-      <c r="K17" s="93" t="s">
-        <v>46</v>
-      </c>
-      <c r="L17" s="93" t="s">
-        <v>46</v>
-      </c>
-      <c r="M17" s="93" t="s">
-        <v>46</v>
-      </c>
-      <c r="N17" s="93" t="s">
-        <v>46</v>
-      </c>
-      <c r="O17" s="94" t="s">
-        <v>46</v>
-      </c>
-      <c r="P17" s="95" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q17" s="93" t="s">
-        <v>116</v>
-      </c>
-      <c r="R17" s="93" t="s">
-        <v>116</v>
-      </c>
-      <c r="S17" s="94" t="s">
-        <v>116</v>
-      </c>
-      <c r="T17" s="96" t="s">
-        <v>132</v>
-      </c>
-      <c r="U17" s="92" t="s">
-        <v>53</v>
-      </c>
-      <c r="V17" s="33" t="s">
+      <c r="F19" s="89"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="91" t="s">
+        <v>132</v>
+      </c>
+      <c r="I19" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="K19" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="L19" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="M19" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="N19" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="O19" s="93" t="s">
+        <v>46</v>
+      </c>
+      <c r="P19" s="94" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q19" s="92" t="s">
+        <v>115</v>
+      </c>
+      <c r="R19" s="92" t="s">
+        <v>115</v>
+      </c>
+      <c r="S19" s="93" t="s">
+        <v>115</v>
+      </c>
+      <c r="T19" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="U19" s="91" t="s">
+        <v>53</v>
+      </c>
+      <c r="V19" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="79">
-        <v>5</v>
-      </c>
-      <c r="B18" s="61" t="s">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A20" s="78">
+        <v>7</v>
+      </c>
+      <c r="B20" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" s="38">
+      <c r="C20" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="38">
         <v>1</v>
       </c>
-      <c r="E18" s="38">
+      <c r="E20" s="38">
         <v>900</v>
       </c>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="40" t="s">
-        <v>133</v>
-      </c>
-      <c r="I18" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="J18" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="K18" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="L18" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="M18" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="N18" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="O18" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="P18" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q18" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="R18" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="S18" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="T18" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="U18" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="V18" s="33" t="s">
+      <c r="F20" s="38"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="I20" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="J20" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="K20" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="L20" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="M20" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="N20" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="O20" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="P20" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q20" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="R20" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="S20" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="T20" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="U20" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="V20" s="33" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="79">
-        <v>6</v>
-      </c>
-      <c r="B19" s="62" t="s">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A21" s="78">
+        <v>8</v>
+      </c>
+      <c r="B21" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="D19" s="45">
-        <v>1</v>
-      </c>
-      <c r="E19" s="45">
-        <v>900</v>
-      </c>
-      <c r="F19" s="45"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="40" t="s">
-        <v>133</v>
-      </c>
-      <c r="I19" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="J19" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="K19" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="L19" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="M19" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="N19" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="O19" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="P19" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q19" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="R19" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="S19" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="T19" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="U19" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="V19" s="33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="79">
-        <v>7</v>
-      </c>
-      <c r="B20" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="D20" s="45">
-        <v>1</v>
-      </c>
-      <c r="E20" s="45">
-        <v>900</v>
-      </c>
-      <c r="F20" s="45"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="40" t="s">
-        <v>133</v>
-      </c>
-      <c r="I20" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="J20" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="K20" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="L20" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="M20" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="N20" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="O20" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="P20" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q20" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="R20" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="S20" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="T20" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="U20" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="V20" s="33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="79">
-        <v>8</v>
-      </c>
-      <c r="B21" s="62" t="s">
-        <v>3</v>
-      </c>
       <c r="C21" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D21" s="45">
         <v>1</v>
@@ -2544,13 +2553,13 @@
       <c r="F21" s="45"/>
       <c r="G21" s="46"/>
       <c r="H21" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I21" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J21" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K21" s="48" t="s">
         <v>46</v>
@@ -2586,21 +2595,21 @@
         <v>53</v>
       </c>
       <c r="V21" s="33" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="79">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A22" s="78">
         <v>9</v>
       </c>
       <c r="B22" s="62" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D22" s="45">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E22" s="45">
         <v>900</v>
@@ -2608,13 +2617,13 @@
       <c r="F22" s="45"/>
       <c r="G22" s="46"/>
       <c r="H22" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I22" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J22" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K22" s="48" t="s">
         <v>46</v>
@@ -2632,36 +2641,36 @@
         <v>46</v>
       </c>
       <c r="P22" s="50" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="Q22" s="48" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="R22" s="48" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="S22" s="49" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="T22" s="44" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="U22" s="47" t="s">
         <v>53</v>
       </c>
       <c r="V22" s="33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="79">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A23" s="78">
         <v>10</v>
       </c>
       <c r="B23" s="62" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D23" s="45">
         <v>1</v>
@@ -2672,13 +2681,13 @@
       <c r="F23" s="45"/>
       <c r="G23" s="46"/>
       <c r="H23" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I23" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J23" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K23" s="48" t="s">
         <v>46</v>
@@ -2696,16 +2705,16 @@
         <v>46</v>
       </c>
       <c r="P23" s="50" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="Q23" s="48" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="R23" s="48" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="S23" s="49" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="T23" s="44" t="s">
         <v>46</v>
@@ -2714,21 +2723,21 @@
         <v>53</v>
       </c>
       <c r="V23" s="33" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="79">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A24" s="78">
         <v>11</v>
       </c>
       <c r="B24" s="62" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D24" s="45">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E24" s="45">
         <v>900</v>
@@ -2736,13 +2745,13 @@
       <c r="F24" s="45"/>
       <c r="G24" s="46"/>
       <c r="H24" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I24" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J24" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K24" s="48" t="s">
         <v>46</v>
@@ -2760,36 +2769,36 @@
         <v>46</v>
       </c>
       <c r="P24" s="50" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="Q24" s="48" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="R24" s="48" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="S24" s="49" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="T24" s="44" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="U24" s="47" t="s">
         <v>53</v>
       </c>
       <c r="V24" s="33" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="79">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A25" s="78">
         <v>12</v>
       </c>
       <c r="B25" s="62" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D25" s="45">
         <v>1</v>
@@ -2800,13 +2809,13 @@
       <c r="F25" s="45"/>
       <c r="G25" s="46"/>
       <c r="H25" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I25" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J25" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K25" s="48" t="s">
         <v>46</v>
@@ -2824,16 +2833,16 @@
         <v>46</v>
       </c>
       <c r="P25" s="50" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="Q25" s="48" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="R25" s="48" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="S25" s="49" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="T25" s="44" t="s">
         <v>46</v>
@@ -2842,18 +2851,18 @@
         <v>53</v>
       </c>
       <c r="V25" s="33" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="79">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A26" s="78">
         <v>13</v>
       </c>
       <c r="B26" s="62" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D26" s="45">
         <v>1</v>
@@ -2864,13 +2873,13 @@
       <c r="F26" s="45"/>
       <c r="G26" s="46"/>
       <c r="H26" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I26" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J26" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K26" s="48" t="s">
         <v>46</v>
@@ -2900,24 +2909,24 @@
         <v>46</v>
       </c>
       <c r="T26" s="44" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="U26" s="47" t="s">
         <v>53</v>
       </c>
       <c r="V26" s="33" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="79">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A27" s="78">
         <v>14</v>
       </c>
       <c r="B27" s="62" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D27" s="45">
         <v>1</v>
@@ -2928,13 +2937,13 @@
       <c r="F27" s="45"/>
       <c r="G27" s="46"/>
       <c r="H27" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I27" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J27" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K27" s="48" t="s">
         <v>46</v>
@@ -2970,21 +2979,21 @@
         <v>53</v>
       </c>
       <c r="V27" s="33" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="79">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A28" s="78">
         <v>15</v>
       </c>
       <c r="B28" s="62" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D28" s="45">
-        <v>900</v>
+        <v>1</v>
       </c>
       <c r="E28" s="45">
         <v>900</v>
@@ -2992,40 +3001,40 @@
       <c r="F28" s="45"/>
       <c r="G28" s="46"/>
       <c r="H28" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I28" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J28" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K28" s="48" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="L28" s="48" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="M28" s="48" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="N28" s="48" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="O28" s="49" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="P28" s="50" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="Q28" s="48" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="R28" s="48" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="S28" s="49" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="T28" s="44" t="s">
         <v>53</v>
@@ -3034,21 +3043,21 @@
         <v>53</v>
       </c>
       <c r="V28" s="33" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="79">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A29" s="78">
         <v>16</v>
       </c>
       <c r="B29" s="62" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D29" s="45">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="E29" s="45">
         <v>900</v>
@@ -3056,13 +3065,13 @@
       <c r="F29" s="45"/>
       <c r="G29" s="46"/>
       <c r="H29" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I29" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J29" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K29" s="48" t="s">
         <v>46</v>
@@ -3083,36 +3092,36 @@
         <v>46</v>
       </c>
       <c r="Q29" s="48" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="R29" s="48" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="S29" s="49" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="T29" s="44" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="U29" s="47" t="s">
         <v>53</v>
       </c>
       <c r="V29" s="33" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="79">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A30" s="78">
         <v>17</v>
       </c>
       <c r="B30" s="62" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D30" s="45">
-        <v>80</v>
+        <v>900</v>
       </c>
       <c r="E30" s="45">
         <v>900</v>
@@ -3120,31 +3129,31 @@
       <c r="F30" s="45"/>
       <c r="G30" s="46"/>
       <c r="H30" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I30" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J30" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K30" s="48" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="L30" s="48" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="M30" s="48" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="N30" s="48" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="O30" s="49" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="P30" s="50" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="Q30" s="48" t="s">
         <v>53</v>
@@ -3162,35 +3171,35 @@
         <v>53</v>
       </c>
       <c r="V30" s="33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="79">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A31" s="78">
         <v>18</v>
       </c>
       <c r="B31" s="62" t="s">
-        <v>109</v>
+        <v>10</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D31" s="45">
         <v>80</v>
       </c>
       <c r="E31" s="45">
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="F31" s="45"/>
       <c r="G31" s="46"/>
       <c r="H31" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I31" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J31" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K31" s="48" t="s">
         <v>46</v>
@@ -3199,7 +3208,7 @@
         <v>46</v>
       </c>
       <c r="M31" s="48" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="N31" s="48" t="s">
         <v>46</v>
@@ -3226,35 +3235,35 @@
         <v>53</v>
       </c>
       <c r="V31" s="33" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="79">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A32" s="78">
         <v>19</v>
       </c>
       <c r="B32" s="62" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D32" s="45">
         <v>80</v>
       </c>
       <c r="E32" s="45">
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="F32" s="45"/>
       <c r="G32" s="46"/>
       <c r="H32" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I32" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J32" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K32" s="48" t="s">
         <v>46</v>
@@ -3263,7 +3272,7 @@
         <v>46</v>
       </c>
       <c r="M32" s="48" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="N32" s="48" t="s">
         <v>46</v>
@@ -3290,18 +3299,18 @@
         <v>53</v>
       </c>
       <c r="V32" s="33" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" s="79">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A33" s="78">
         <v>20</v>
       </c>
       <c r="B33" s="62" t="s">
-        <v>92</v>
+        <v>157</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D33" s="45">
         <v>80</v>
@@ -3312,13 +3321,13 @@
       <c r="F33" s="45"/>
       <c r="G33" s="46"/>
       <c r="H33" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I33" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J33" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K33" s="48" t="s">
         <v>46</v>
@@ -3327,7 +3336,7 @@
         <v>46</v>
       </c>
       <c r="M33" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N33" s="48" t="s">
         <v>46</v>
@@ -3354,18 +3363,18 @@
         <v>53</v>
       </c>
       <c r="V33" s="33" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A34" s="79">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A34" s="78">
         <v>21</v>
       </c>
       <c r="B34" s="62" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D34" s="45">
         <v>80</v>
@@ -3376,13 +3385,13 @@
       <c r="F34" s="45"/>
       <c r="G34" s="46"/>
       <c r="H34" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I34" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J34" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K34" s="48" t="s">
         <v>46</v>
@@ -3391,7 +3400,7 @@
         <v>46</v>
       </c>
       <c r="M34" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N34" s="48" t="s">
         <v>46</v>
@@ -3418,18 +3427,18 @@
         <v>53</v>
       </c>
       <c r="V34" s="33" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A35" s="79">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A35" s="78">
         <v>22</v>
       </c>
       <c r="B35" s="62" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D35" s="45">
         <v>80</v>
@@ -3440,13 +3449,13 @@
       <c r="F35" s="45"/>
       <c r="G35" s="46"/>
       <c r="H35" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I35" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J35" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K35" s="48" t="s">
         <v>46</v>
@@ -3455,7 +3464,7 @@
         <v>46</v>
       </c>
       <c r="M35" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N35" s="48" t="s">
         <v>46</v>
@@ -3482,18 +3491,18 @@
         <v>53</v>
       </c>
       <c r="V35" s="33" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A36" s="79">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A36" s="78">
         <v>23</v>
       </c>
       <c r="B36" s="62" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D36" s="45">
         <v>80</v>
@@ -3504,13 +3513,13 @@
       <c r="F36" s="45"/>
       <c r="G36" s="46"/>
       <c r="H36" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I36" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J36" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K36" s="48" t="s">
         <v>46</v>
@@ -3519,7 +3528,7 @@
         <v>46</v>
       </c>
       <c r="M36" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N36" s="48" t="s">
         <v>46</v>
@@ -3546,18 +3555,18 @@
         <v>53</v>
       </c>
       <c r="V36" s="33" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A37" s="79">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A37" s="78">
         <v>24</v>
       </c>
       <c r="B37" s="62" t="s">
-        <v>111</v>
+        <v>7</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D37" s="45">
         <v>80</v>
@@ -3568,13 +3577,13 @@
       <c r="F37" s="45"/>
       <c r="G37" s="46"/>
       <c r="H37" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I37" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J37" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K37" s="48" t="s">
         <v>46</v>
@@ -3583,7 +3592,7 @@
         <v>46</v>
       </c>
       <c r="M37" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N37" s="48" t="s">
         <v>46</v>
@@ -3610,167 +3619,167 @@
         <v>53</v>
       </c>
       <c r="V37" s="33" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A38" s="79">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A38" s="78">
         <v>25</v>
       </c>
-      <c r="B38" s="63" t="s">
+      <c r="B38" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="D38" s="45">
+        <v>80</v>
+      </c>
+      <c r="E38" s="45">
+        <v>600</v>
+      </c>
+      <c r="F38" s="45"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="I38" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="J38" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="K38" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="L38" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="M38" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="N38" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="O38" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="P38" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q38" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="R38" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="S38" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="T38" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="U38" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="V38" s="33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A39" s="78">
+        <v>26</v>
+      </c>
+      <c r="B39" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" s="45">
+        <v>80</v>
+      </c>
+      <c r="E39" s="45">
+        <v>600</v>
+      </c>
+      <c r="F39" s="45"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="I39" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="J39" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="K39" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="L39" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="M39" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="N39" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="O39" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="P39" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q39" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="R39" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="S39" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="T39" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="U39" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="V39" s="33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A40" s="78">
+        <v>27</v>
+      </c>
+      <c r="B40" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="D38" s="26">
+      <c r="C40" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D40" s="26">
         <v>1</v>
-      </c>
-      <c r="E38" s="26">
-        <v>1</v>
-      </c>
-      <c r="F38" s="26">
-        <v>100</v>
-      </c>
-      <c r="G38" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="H38" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N38" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O38" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="P38" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q38" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="R38" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="S38" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="T38" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="U38" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="V38" s="33" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A39" s="79">
-        <v>26</v>
-      </c>
-      <c r="B39" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="D39" s="26">
-        <v>100</v>
-      </c>
-      <c r="E39" s="26">
-        <v>1</v>
-      </c>
-      <c r="F39" s="26"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N39" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O39" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P39" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q39" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="R39" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="S39" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="T39" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="U39" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="V39" s="33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A40" s="79">
-        <v>27</v>
-      </c>
-      <c r="B40" s="64" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="26">
-        <v>100</v>
       </c>
       <c r="E40" s="26">
         <v>1</v>
       </c>
-      <c r="F40" s="7"/>
-      <c r="G40" s="8"/>
+      <c r="F40" s="26">
+        <v>100</v>
+      </c>
+      <c r="G40" s="27" t="s">
+        <v>50</v>
+      </c>
       <c r="H40" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>46</v>
@@ -3785,332 +3794,332 @@
         <v>46</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>46</v>
+        <v>136</v>
       </c>
       <c r="P40" s="21" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>53</v>
+        <v>148</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="S40" s="3" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="T40" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U40" s="23" t="s">
         <v>53</v>
       </c>
       <c r="V40" s="33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41" s="79">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A41" s="78">
         <v>28</v>
       </c>
       <c r="B41" s="63" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="C41" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D41" s="26">
+        <v>100</v>
+      </c>
+      <c r="E41" s="26">
+        <v>1</v>
+      </c>
+      <c r="F41" s="26"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O41" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P41" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R41" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S41" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T41" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="U41" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="V41" s="33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A42" s="78">
+        <v>29</v>
+      </c>
+      <c r="B42" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="26">
+      <c r="D42" s="26">
+        <v>100</v>
+      </c>
+      <c r="E42" s="26">
         <v>1</v>
-      </c>
-      <c r="E41" s="26">
-        <v>500</v>
-      </c>
-      <c r="F41" s="26"/>
-      <c r="G41" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="H41" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="N41" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="O41" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P41" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q41" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="R41" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="S41" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="T41" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="U41" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="V41" s="33" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42" s="79">
-        <v>29</v>
-      </c>
-      <c r="B42" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="D42" s="7">
-        <v>20</v>
-      </c>
-      <c r="E42" s="7">
-        <v>60</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
       <c r="H42" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="O42" s="2" t="s">
-        <v>133</v>
+        <v>46</v>
+      </c>
+      <c r="O42" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="P42" s="21" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>136</v>
+        <v>53</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="S42" s="3" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="T42" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U42" s="23" t="s">
         <v>53</v>
       </c>
       <c r="V42" s="33" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43" s="79">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A43" s="78">
         <v>30</v>
       </c>
       <c r="B43" s="63" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="C43" s="29" t="s">
         <v>47</v>
       </c>
       <c r="D43" s="26">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="E43" s="26">
         <v>500</v>
       </c>
       <c r="F43" s="26"/>
-      <c r="G43" s="27"/>
+      <c r="G43" s="27" t="s">
+        <v>48</v>
+      </c>
       <c r="H43" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O43" s="3" t="s">
         <v>46</v>
       </c>
       <c r="P43" s="21" t="s">
-        <v>141</v>
+        <v>46</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="R43" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="T43" s="13" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="U43" s="23" t="s">
         <v>53</v>
       </c>
       <c r="V43" s="33" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A44" s="79">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A44" s="78">
         <v>31</v>
       </c>
-      <c r="B44" s="63" t="s">
-        <v>11</v>
+      <c r="B44" s="64" t="s">
+        <v>78</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="D44" s="26">
+        <v>150</v>
+      </c>
+      <c r="D44" s="7">
+        <v>20</v>
+      </c>
+      <c r="E44" s="7">
+        <v>60</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="P44" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="R44" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="S44" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="T44" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="U44" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="V44" s="33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A45" s="78">
+        <v>32</v>
+      </c>
+      <c r="B45" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="26">
         <v>80</v>
       </c>
-      <c r="E44" s="26">
-        <v>1100</v>
-      </c>
-      <c r="F44" s="26"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N44" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O44" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P44" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q44" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="R44" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="S44" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="T44" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U44" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="V44" s="33" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A45" s="79">
-        <v>32</v>
-      </c>
-      <c r="B45" s="63" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="D45" s="26">
-        <v>1</v>
-      </c>
       <c r="E45" s="26">
-        <v>1100</v>
+        <v>500</v>
       </c>
       <c r="F45" s="26"/>
       <c r="G45" s="27"/>
       <c r="H45" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="O45" s="3" t="s">
         <v>46</v>
       </c>
       <c r="P45" s="21" t="s">
-        <v>53</v>
+        <v>140</v>
       </c>
       <c r="Q45" s="2" t="s">
         <v>53</v>
@@ -4122,149 +4131,149 @@
         <v>53</v>
       </c>
       <c r="T45" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="U45" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="V45" s="33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A46" s="78">
+        <v>33</v>
+      </c>
+      <c r="B46" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" s="26">
+        <v>80</v>
+      </c>
+      <c r="E46" s="26">
+        <v>1100</v>
+      </c>
+      <c r="F46" s="26"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O46" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P46" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R46" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S46" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T46" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="U46" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="V46" s="33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A47" s="78">
+        <v>34</v>
+      </c>
+      <c r="B47" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="U45" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="V45" s="33" t="s">
+      <c r="D47" s="26">
+        <v>1</v>
+      </c>
+      <c r="E47" s="26">
+        <v>1100</v>
+      </c>
+      <c r="F47" s="26"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O47" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P47" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S47" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T47" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="U47" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="V47" s="33" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A46" s="79">
-        <v>33</v>
-      </c>
-      <c r="B46" s="64" t="s">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A48" s="78">
+        <v>35</v>
+      </c>
+      <c r="B48" s="64" t="s">
         <v>17</v>
-      </c>
-      <c r="C46" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D46" s="7">
-        <v>1</v>
-      </c>
-      <c r="E46" s="7">
-        <v>100</v>
-      </c>
-      <c r="F46" s="7"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="L46" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="N46" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="O46" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="P46" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q46" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="R46" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="S46" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="T46" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="U46" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="V46" s="33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A47" s="79">
-        <v>34</v>
-      </c>
-      <c r="B47" s="64" t="s">
-        <v>79</v>
-      </c>
-      <c r="C47" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" s="7">
-        <v>50</v>
-      </c>
-      <c r="E47" s="7">
-        <v>60</v>
-      </c>
-      <c r="F47" s="7"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N47" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O47" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P47" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q47" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="R47" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="S47" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="T47" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U47" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="V47" s="33" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A48" s="79">
-        <v>35</v>
-      </c>
-      <c r="B48" s="64" t="s">
-        <v>19</v>
       </c>
       <c r="C48" s="29" t="s">
         <v>47</v>
@@ -4273,68 +4282,68 @@
         <v>1</v>
       </c>
       <c r="E48" s="7">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
       <c r="H48" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="P48" s="21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="R48" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T48" s="13" t="s">
-        <v>46</v>
+        <v>134</v>
       </c>
       <c r="U48" s="23" t="s">
         <v>53</v>
       </c>
       <c r="V48" s="33" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A49" s="79">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A49" s="78">
         <v>36</v>
       </c>
       <c r="B49" s="64" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C49" s="29" t="s">
         <v>47</v>
       </c>
       <c r="D49" s="7">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E49" s="7">
         <v>60</v>
@@ -4342,10 +4351,10 @@
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
       <c r="H49" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>46</v>
@@ -4366,16 +4375,16 @@
         <v>46</v>
       </c>
       <c r="P49" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="S49" s="3" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="T49" s="13" t="s">
         <v>53</v>
@@ -4384,35 +4393,35 @@
         <v>53</v>
       </c>
       <c r="V49" s="33" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A50" s="79">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A50" s="78">
         <v>37</v>
       </c>
       <c r="B50" s="64" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C50" s="29" t="s">
         <v>47</v>
       </c>
       <c r="D50" s="7">
+        <v>1</v>
+      </c>
+      <c r="E50" s="7">
         <v>20</v>
-      </c>
-      <c r="E50" s="7">
-        <v>60</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
       <c r="H50" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>46</v>
@@ -4430,39 +4439,39 @@
         <v>46</v>
       </c>
       <c r="P50" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q50" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R50" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S50" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T50" s="13" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="U50" s="23" t="s">
         <v>53</v>
       </c>
       <c r="V50" s="33" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A51" s="79">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A51" s="78">
         <v>38</v>
       </c>
       <c r="B51" s="64" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C51" s="29" t="s">
         <v>47</v>
       </c>
       <c r="D51" s="7">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E51" s="7">
         <v>60</v>
@@ -4470,13 +4479,13 @@
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
       <c r="H51" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="K51" s="2" t="s">
         <v>46</v>
@@ -4485,59 +4494,59 @@
         <v>46</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="P51" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R51" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S51" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T51" s="13" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="U51" s="23" t="s">
         <v>53</v>
       </c>
       <c r="V51" s="33" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A52" s="79">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A52" s="78">
         <v>39</v>
       </c>
       <c r="B52" s="64" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C52" s="29" t="s">
         <v>47</v>
       </c>
       <c r="D52" s="7">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E52" s="7">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
       <c r="H52" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>46</v>
@@ -4558,53 +4567,53 @@
         <v>46</v>
       </c>
       <c r="P52" s="21" t="s">
-        <v>46</v>
+        <v>142</v>
       </c>
       <c r="Q52" s="2" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="R52" s="2" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="S52" s="3" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="T52" s="13" t="s">
-        <v>135</v>
+        <v>53</v>
       </c>
       <c r="U52" s="23" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="V52" s="33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A53" s="79">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A53" s="78">
         <v>40</v>
       </c>
       <c r="B53" s="64" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C53" s="29" t="s">
         <v>47</v>
       </c>
       <c r="D53" s="7">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E53" s="7">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
       <c r="H53" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="K53" s="2" t="s">
         <v>46</v>
@@ -4613,48 +4622,48 @@
         <v>46</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="O53" s="3" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="P53" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q53" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R53" s="2" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T53" s="13" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="U53" s="23" t="s">
         <v>53</v>
       </c>
       <c r="V53" s="33" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A54" s="79">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A54" s="78">
         <v>41</v>
       </c>
       <c r="B54" s="64" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C54" s="29" t="s">
         <v>47</v>
       </c>
       <c r="D54" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54" s="7">
         <v>1</v>
@@ -4662,10 +4671,10 @@
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
       <c r="H54" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>46</v>
@@ -4698,35 +4707,35 @@
         <v>46</v>
       </c>
       <c r="T54" s="13" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="U54" s="23" t="s">
         <v>46</v>
       </c>
       <c r="V54" s="33" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A55" s="79">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A55" s="78">
         <v>42</v>
       </c>
       <c r="B55" s="64" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C55" s="29" t="s">
         <v>47</v>
       </c>
       <c r="D55" s="7">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E55" s="7">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
       <c r="H55" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>46</v>
@@ -4750,50 +4759,50 @@
         <v>46</v>
       </c>
       <c r="P55" s="21" t="s">
-        <v>46</v>
+        <v>142</v>
       </c>
       <c r="Q55" s="2" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="R55" s="2" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="T55" s="13" t="s">
-        <v>135</v>
+        <v>53</v>
       </c>
       <c r="U55" s="23" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="V55" s="33" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A56" s="79">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A56" s="78">
         <v>43</v>
       </c>
-      <c r="B56" s="65" t="s">
-        <v>64</v>
+      <c r="B56" s="64" t="s">
+        <v>27</v>
       </c>
       <c r="C56" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D56" s="30">
-        <v>40</v>
-      </c>
-      <c r="E56" s="30">
-        <v>600</v>
-      </c>
-      <c r="F56" s="30"/>
-      <c r="G56" s="31"/>
+      <c r="D56" s="7">
+        <v>1</v>
+      </c>
+      <c r="E56" s="7">
+        <v>1</v>
+      </c>
+      <c r="F56" s="7"/>
+      <c r="G56" s="8"/>
       <c r="H56" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>46</v>
@@ -4805,7 +4814,7 @@
         <v>46</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="N56" s="2" t="s">
         <v>46</v>
@@ -4814,50 +4823,50 @@
         <v>46</v>
       </c>
       <c r="P56" s="21" t="s">
-        <v>141</v>
+        <v>46</v>
       </c>
       <c r="Q56" s="2" t="s">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="S56" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="T56" s="13" t="s">
-        <v>53</v>
+        <v>152</v>
       </c>
       <c r="U56" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="V56" s="34" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A57" s="79">
+        <v>46</v>
+      </c>
+      <c r="V56" s="33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A57" s="78">
         <v>44</v>
       </c>
       <c r="B57" s="64" t="s">
-        <v>107</v>
+        <v>28</v>
       </c>
       <c r="C57" s="29" t="s">
         <v>47</v>
       </c>
       <c r="D57" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57" s="7">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
       <c r="H57" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>46</v>
@@ -4878,10 +4887,10 @@
         <v>46</v>
       </c>
       <c r="P57" s="21" t="s">
-        <v>144</v>
+        <v>46</v>
       </c>
       <c r="Q57" s="2" t="s">
-        <v>150</v>
+        <v>46</v>
       </c>
       <c r="R57" s="2" t="s">
         <v>46</v>
@@ -4890,102 +4899,268 @@
         <v>46</v>
       </c>
       <c r="T57" s="13" t="s">
-        <v>46</v>
+        <v>152</v>
       </c>
       <c r="U57" s="23" t="s">
         <v>46</v>
       </c>
       <c r="V57" s="33" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A58" s="79">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A58" s="78">
         <v>45</v>
       </c>
       <c r="B58" s="65" t="s">
-        <v>152</v>
-      </c>
-      <c r="C58" s="82" t="s">
-        <v>125</v>
+        <v>64</v>
+      </c>
+      <c r="C58" s="29" t="s">
+        <v>47</v>
       </c>
       <c r="D58" s="30">
-        <v>700</v>
+        <v>40</v>
       </c>
       <c r="E58" s="30">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="F58" s="30"/>
       <c r="G58" s="31"/>
       <c r="H58" s="23" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>148</v>
+        <v>46</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="L58" s="84" t="s">
-        <v>46</v>
-      </c>
-      <c r="M58" s="84" t="s">
-        <v>53</v>
-      </c>
-      <c r="N58" s="84" t="s">
-        <v>53</v>
-      </c>
-      <c r="O58" s="85" t="s">
-        <v>53</v>
-      </c>
-      <c r="P58" s="86" t="s">
+        <v>46</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N58" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O58" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P58" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q58" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="R58" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S58" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T58" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="U58" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="V58" s="34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A59" s="78">
+        <v>46</v>
+      </c>
+      <c r="B59" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="C59" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59" s="7">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7">
+        <v>60</v>
+      </c>
+      <c r="F59" s="7"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N59" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O59" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P59" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q59" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="R59" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S59" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T59" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="U59" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="V59" s="33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A60" s="78">
+        <v>47</v>
+      </c>
+      <c r="B60" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="C60" s="81" t="s">
+        <v>124</v>
+      </c>
+      <c r="D60" s="30">
+        <v>700</v>
+      </c>
+      <c r="E60" s="30">
+        <v>800</v>
+      </c>
+      <c r="F60" s="30"/>
+      <c r="G60" s="31"/>
+      <c r="H60" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="Q58" s="84" t="s">
-        <v>53</v>
-      </c>
-      <c r="R58" s="84" t="s">
-        <v>53</v>
-      </c>
-      <c r="S58" s="85" t="s">
-        <v>53</v>
-      </c>
-      <c r="T58" s="87" t="s">
-        <v>53</v>
-      </c>
-      <c r="U58" s="83" t="s">
-        <v>53</v>
-      </c>
-      <c r="V58" s="34" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="59" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="80"/>
-      <c r="B59" s="66"/>
-      <c r="C59" s="81"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="10"/>
-      <c r="H59" s="24"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="O59" s="5"/>
-      <c r="P59" s="22"/>
-      <c r="Q59" s="4"/>
-      <c r="R59" s="4"/>
-      <c r="S59" s="5"/>
-      <c r="T59" s="6"/>
-      <c r="U59" s="24"/>
-      <c r="V59" s="35"/>
+      <c r="I60" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="L60" s="83" t="s">
+        <v>46</v>
+      </c>
+      <c r="M60" s="83" t="s">
+        <v>53</v>
+      </c>
+      <c r="N60" s="83" t="s">
+        <v>53</v>
+      </c>
+      <c r="O60" s="84" t="s">
+        <v>53</v>
+      </c>
+      <c r="P60" s="85" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q60" s="83" t="s">
+        <v>53</v>
+      </c>
+      <c r="R60" s="83" t="s">
+        <v>53</v>
+      </c>
+      <c r="S60" s="84" t="s">
+        <v>53</v>
+      </c>
+      <c r="T60" s="86" t="s">
+        <v>53</v>
+      </c>
+      <c r="U60" s="82" t="s">
+        <v>53</v>
+      </c>
+      <c r="V60" s="34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="79">
+        <v>48</v>
+      </c>
+      <c r="B61" s="66" t="s">
+        <v>155</v>
+      </c>
+      <c r="C61" s="80" t="s">
+        <v>156</v>
+      </c>
+      <c r="D61" s="9">
+        <v>0</v>
+      </c>
+      <c r="E61" s="9">
+        <v>1</v>
+      </c>
+      <c r="F61" s="9"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L61" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M61" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N61" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O61" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="P61" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q61" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R61" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S61" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="T61" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="U61" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="V61" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>